<commit_message>
new numbers and stuff
</commit_message>
<xml_diff>
--- a/report/anything else/equation.xlsx
+++ b/report/anything else/equation.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
   <si>
     <t>Input signal</t>
   </si>
@@ -82,6 +82,24 @@
   </si>
   <si>
     <t>micros-761</t>
+  </si>
+  <si>
+    <t>NEWEST DATA</t>
+  </si>
+  <si>
+    <t>Microsecons</t>
+  </si>
+  <si>
+    <t>Motor1 RPM</t>
+  </si>
+  <si>
+    <t>Motor2 RPM</t>
+  </si>
+  <si>
+    <t>Motor3 RPM</t>
+  </si>
+  <si>
+    <t>Motor4 RPM</t>
   </si>
 </sst>
 </file>
@@ -510,11 +528,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="58824192"/>
-        <c:axId val="58825728"/>
+        <c:axId val="84715008"/>
+        <c:axId val="84716544"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="58824192"/>
+        <c:axId val="84715008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1200"/>
@@ -527,12 +545,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58825728"/>
+        <c:crossAx val="84716544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="58825728"/>
+        <c:axId val="84716544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10261"/>
@@ -545,14 +563,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58824192"/>
+        <c:crossAx val="84715008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -582,7 +599,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -832,11 +848,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="67181184"/>
-        <c:axId val="67191168"/>
+        <c:axId val="85531264"/>
+        <c:axId val="85541248"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="67181184"/>
+        <c:axId val="85531264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1200"/>
@@ -848,12 +864,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67191168"/>
+        <c:crossAx val="85541248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="67191168"/>
+        <c:axId val="85541248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10261"/>
@@ -866,7 +882,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67181184"/>
+        <c:crossAx val="85531264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -912,7 +928,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1162,11 +1177,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="67212416"/>
-        <c:axId val="67213952"/>
+        <c:axId val="85570688"/>
+        <c:axId val="85572224"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="67212416"/>
+        <c:axId val="85570688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1200"/>
@@ -1178,12 +1193,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67213952"/>
+        <c:crossAx val="85572224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="67213952"/>
+        <c:axId val="85572224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10260"/>
@@ -1196,7 +1211,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67212416"/>
+        <c:crossAx val="85570688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1377,11 +1392,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="77011584"/>
-        <c:axId val="77017472"/>
+        <c:axId val="88287872"/>
+        <c:axId val="88293760"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="77011584"/>
+        <c:axId val="88287872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1391,12 +1406,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77017472"/>
+        <c:crossAx val="88293760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="77017472"/>
+        <c:axId val="88293760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1407,7 +1422,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77011584"/>
+        <c:crossAx val="88287872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1567,11 +1582,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="77051008"/>
-        <c:axId val="77052544"/>
+        <c:axId val="88308352"/>
+        <c:axId val="88326528"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="77051008"/>
+        <c:axId val="88308352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1581,12 +1596,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77052544"/>
+        <c:crossAx val="88326528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="77052544"/>
+        <c:axId val="88326528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1597,7 +1612,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77051008"/>
+        <c:crossAx val="88308352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1635,7 +1650,17 @@
   <c:chart>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="4.836462343615499E-2"/>
+          <c:y val="3.75116652085156E-2"/>
+          <c:w val="0.78869732832691686"/>
+          <c:h val="0.8326195683872849"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
@@ -1648,62 +1673,32 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:trendline>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-0.59869843734321937"/>
-                  <c:y val="-6.5289442986293383E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:pPr>
-                      <a:defRPr/>
-                    </a:pPr>
-                    <a:r>
-                      <a:rPr lang="en-GB" baseline="0"/>
-                      <a:t>M1 = 0.0585x + 1042.8</a:t>
-                    </a:r>
-                    <a:endParaRPr lang="en-GB"/>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-            </c:trendlineLbl>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$O$82:$O$88</c:f>
+              <c:f>Sheet1!$A$82:$A$88</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>739</c:v>
+                  <c:v>1500</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>789</c:v>
+                  <c:v>1550</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>839</c:v>
+                  <c:v>1600</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>889</c:v>
+                  <c:v>1650</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>939</c:v>
+                  <c:v>1700</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>989</c:v>
+                  <c:v>1750</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1039</c:v>
+                  <c:v>1800</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1749,62 +1744,32 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:trendline>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-0.43639126095153596"/>
-                  <c:y val="-0.15259405074365703"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:pPr>
-                      <a:defRPr/>
-                    </a:pPr>
-                    <a:r>
-                      <a:rPr lang="en-GB" baseline="0"/>
-                      <a:t>M2 = 0.0676x + 1015.8</a:t>
-                    </a:r>
-                    <a:endParaRPr lang="en-GB"/>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-            </c:trendlineLbl>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$O$82:$O$88</c:f>
+              <c:f>Sheet1!$A$82:$A$88</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>739</c:v>
+                  <c:v>1500</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>789</c:v>
+                  <c:v>1550</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>839</c:v>
+                  <c:v>1600</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>889</c:v>
+                  <c:v>1650</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>939</c:v>
+                  <c:v>1700</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>989</c:v>
+                  <c:v>1750</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1039</c:v>
+                  <c:v>1800</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1853,59 +1818,34 @@
           <c:trendline>
             <c:trendlineType val="linear"/>
             <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-0.24993921534456082"/>
-                  <c:y val="-7.4548702245552642E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:pPr>
-                      <a:defRPr/>
-                    </a:pPr>
-                    <a:r>
-                      <a:rPr lang="en-GB" baseline="0"/>
-                      <a:t>M3 = 0.0643x + 1036.6</a:t>
-                    </a:r>
-                    <a:endParaRPr lang="en-GB"/>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-            </c:trendlineLbl>
+            <c:dispEq val="0"/>
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$O$82:$O$88</c:f>
+              <c:f>Sheet1!$A$82:$A$88</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>739</c:v>
+                  <c:v>1500</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>789</c:v>
+                  <c:v>1550</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>839</c:v>
+                  <c:v>1600</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>889</c:v>
+                  <c:v>1650</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>939</c:v>
+                  <c:v>1700</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>989</c:v>
+                  <c:v>1750</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1039</c:v>
+                  <c:v>1800</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1951,62 +1891,32 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:trendline>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-7.7699055223730842E-2"/>
-                  <c:y val="-0.22354330708661418"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:pPr>
-                      <a:defRPr/>
-                    </a:pPr>
-                    <a:r>
-                      <a:rPr lang="en-GB" baseline="0"/>
-                      <a:t>M4 = 0.0691x + 1007</a:t>
-                    </a:r>
-                    <a:endParaRPr lang="en-GB"/>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-            </c:trendlineLbl>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$O$82:$O$88</c:f>
+              <c:f>Sheet1!$A$82:$A$88</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>739</c:v>
+                  <c:v>1500</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>789</c:v>
+                  <c:v>1550</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>839</c:v>
+                  <c:v>1600</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>889</c:v>
+                  <c:v>1650</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>939</c:v>
+                  <c:v>1700</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>989</c:v>
+                  <c:v>1750</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1039</c:v>
+                  <c:v>1800</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2051,15 +1961,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="60127104"/>
-        <c:axId val="60125568"/>
+        <c:axId val="90333184"/>
+        <c:axId val="90334720"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="60127104"/>
+        <c:axId val="90333184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1039"/>
-          <c:min val="739"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -2067,16 +1975,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="60125568"/>
+        <c:crossAx val="90334720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="60125568"/>
+        <c:axId val="90334720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1105"/>
-          <c:min val="1000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2085,7 +1991,495 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="60127104"/>
+        <c:crossAx val="90333184"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Motor 1</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.33094631659788509"/>
+                  <c:y val="-1.0433019837883337E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr/>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>M3= 0.0562x + 1064.7</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$120:$A$126</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1700</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1900</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$120:$C$126</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1151.3937075406591</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1160.5043262360696</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1167.729989339326</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1173.6990153811466</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1178.4114043615314</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1182.2860353009589</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1185.7417872199076</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Motor 2</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.46776660955965715"/>
+                  <c:y val="-0.21279367526305631"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr/>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>M2 = 0.0571x + 1041.2</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$120:$A$126</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1700</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1900</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$120:$F$126</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1129.61199847577</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1138.513177660941</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1145.8435605193174</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1151.707866806018</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1156.629695296642</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1160.713765746309</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1164.4836769306166</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Motor 3</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.61210387286798151"/>
+                  <c:y val="-1.0433019837883337E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr/>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>M1 = 0.0611x + 1049.5</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$120:$A$126</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1700</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1900</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$I$120:$I$126</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1143.5397259066847</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1154.0117014186508</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1162.3892818282234</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1168.1488683598047</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1173.0706968504287</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1177.5736463205742</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1181.3435575048818</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Motor 4</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.18766657383261176"/>
+                  <c:y val="-0.32358751628090726"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr/>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>M4 = 0.0622x + 1020.7</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$120:$A$126</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1700</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1900</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$L$120:$L$126</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1116.7314685960519</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1126.784565087539</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1134.6385467215136</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1141.1311715389324</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1146.3671592949154</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1150.7653890099414</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1154.8494594596079</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="90393216"/>
+        <c:axId val="90395008"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="90393216"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="2200"/>
+          <c:min val="1600"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="90395008"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="90395008"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1186"/>
+          <c:min val="1116"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="90393216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2262,14 +2656,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>88</xdr:row>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>98</xdr:row>
       <xdr:rowOff>185737</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>103</xdr:row>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>113</xdr:row>
       <xdr:rowOff>71437</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2284,6 +2678,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>19049</xdr:colOff>
+      <xdr:row>128</xdr:row>
+      <xdr:rowOff>80961</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>19049</xdr:colOff>
+      <xdr:row>148</xdr:row>
+      <xdr:rowOff>47624</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2579,10 +3003,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S88"/>
+  <dimension ref="A1:W128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R86" sqref="R86"/>
+    <sheetView tabSelected="1" topLeftCell="A110" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O127" sqref="O127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3504,7 +3928,7 @@
         <v>1074.3199677725895</v>
       </c>
       <c r="D80">
-        <f t="shared" si="5"/>
+        <f>C80/(A80-761)</f>
         <v>1.6812519057474014</v>
       </c>
       <c r="E80">
@@ -3967,6 +4391,824 @@
       <c r="O88">
         <f t="shared" si="12"/>
         <v>1039</v>
+      </c>
+    </row>
+    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>1500</v>
+      </c>
+      <c r="C90">
+        <f t="shared" ref="C90:C96" si="13">A90*0.0585+998.29</f>
+        <v>1086.04</v>
+      </c>
+      <c r="D90">
+        <f>C90/(A90-761)</f>
+        <v>1.4696075778078483</v>
+      </c>
+      <c r="F90">
+        <f>A90*0.0676+964.33</f>
+        <v>1065.73</v>
+      </c>
+      <c r="I90">
+        <f>A90*0.0643+987.67</f>
+        <v>1084.1199999999999</v>
+      </c>
+      <c r="L90">
+        <f>A90*0.0691+954.45</f>
+        <v>1058.1000000000001</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>1550</v>
+      </c>
+      <c r="C91">
+        <f t="shared" si="13"/>
+        <v>1088.9649999999999</v>
+      </c>
+      <c r="D91">
+        <f t="shared" ref="D91:D96" si="14">C91/(A91-761)</f>
+        <v>1.3801837769328262</v>
+      </c>
+      <c r="F91">
+        <f t="shared" ref="F91:F96" si="15">A91*0.0676+964.33</f>
+        <v>1069.1100000000001</v>
+      </c>
+      <c r="I91">
+        <f t="shared" ref="I91:I96" si="16">A91*0.0643+987.67</f>
+        <v>1087.335</v>
+      </c>
+      <c r="L91">
+        <f t="shared" ref="L91:L96" si="17">A91*0.0691+954.45</f>
+        <v>1061.5550000000001</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>1600</v>
+      </c>
+      <c r="C92">
+        <f t="shared" si="13"/>
+        <v>1091.8899999999999</v>
+      </c>
+      <c r="D92">
+        <f t="shared" si="14"/>
+        <v>1.3014183551847436</v>
+      </c>
+      <c r="F92">
+        <f t="shared" si="15"/>
+        <v>1072.49</v>
+      </c>
+      <c r="I92">
+        <f t="shared" si="16"/>
+        <v>1090.55</v>
+      </c>
+      <c r="L92">
+        <f t="shared" si="17"/>
+        <v>1065.01</v>
+      </c>
+    </row>
+    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>1650</v>
+      </c>
+      <c r="C93">
+        <f t="shared" si="13"/>
+        <v>1094.8150000000001</v>
+      </c>
+      <c r="D93">
+        <f t="shared" si="14"/>
+        <v>1.2315129358830146</v>
+      </c>
+      <c r="F93">
+        <f t="shared" si="15"/>
+        <v>1075.8700000000001</v>
+      </c>
+      <c r="I93">
+        <f t="shared" si="16"/>
+        <v>1093.7649999999999</v>
+      </c>
+      <c r="L93">
+        <f t="shared" si="17"/>
+        <v>1068.4650000000001</v>
+      </c>
+    </row>
+    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>1700</v>
+      </c>
+      <c r="C94">
+        <f t="shared" si="13"/>
+        <v>1097.74</v>
+      </c>
+      <c r="D94">
+        <f t="shared" si="14"/>
+        <v>1.1690521831735889</v>
+      </c>
+      <c r="F94">
+        <f t="shared" si="15"/>
+        <v>1079.25</v>
+      </c>
+      <c r="I94">
+        <f t="shared" si="16"/>
+        <v>1096.98</v>
+      </c>
+      <c r="L94">
+        <f t="shared" si="17"/>
+        <v>1071.92</v>
+      </c>
+    </row>
+    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>1750</v>
+      </c>
+      <c r="C95">
+        <f t="shared" si="13"/>
+        <v>1100.665</v>
+      </c>
+      <c r="D95">
+        <f t="shared" si="14"/>
+        <v>1.1129069767441859</v>
+      </c>
+      <c r="F95">
+        <f t="shared" si="15"/>
+        <v>1082.6300000000001</v>
+      </c>
+      <c r="I95">
+        <f t="shared" si="16"/>
+        <v>1100.1949999999999</v>
+      </c>
+      <c r="L95">
+        <f t="shared" si="17"/>
+        <v>1075.375</v>
+      </c>
+    </row>
+    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>1800</v>
+      </c>
+      <c r="C96">
+        <f t="shared" si="13"/>
+        <v>1103.5899999999999</v>
+      </c>
+      <c r="D96">
+        <f t="shared" si="14"/>
+        <v>1.0621655437921078</v>
+      </c>
+      <c r="F96">
+        <f t="shared" si="15"/>
+        <v>1086.01</v>
+      </c>
+      <c r="I96">
+        <f t="shared" si="16"/>
+        <v>1103.4099999999999</v>
+      </c>
+      <c r="L96">
+        <f t="shared" si="17"/>
+        <v>1078.83</v>
+      </c>
+    </row>
+    <row r="98" spans="15:23" x14ac:dyDescent="0.25">
+      <c r="P98">
+        <v>1593</v>
+      </c>
+      <c r="Q98">
+        <v>1609</v>
+      </c>
+    </row>
+    <row r="100" spans="15:23" x14ac:dyDescent="0.25">
+      <c r="O100">
+        <v>1092</v>
+      </c>
+      <c r="P100">
+        <f>(O100-800.801940709803)/0.0585</f>
+        <v>4977.7446032512298</v>
+      </c>
+      <c r="R100">
+        <f>(O100-964.33)/0.0676</f>
+        <v>1888.6094674556209</v>
+      </c>
+      <c r="S100">
+        <f>R100/P100</f>
+        <v>0.37941068053633559</v>
+      </c>
+      <c r="T100">
+        <f>(O100-987.67)/0.0643</f>
+        <v>1622.5505443234845</v>
+      </c>
+      <c r="U100">
+        <f>T100/P100</f>
+        <v>0.32596098708312804</v>
+      </c>
+      <c r="V100">
+        <f>(O100-954.45)/0.0691</f>
+        <v>1990.5933429811862</v>
+      </c>
+      <c r="W100">
+        <f>V100/P100</f>
+        <v>0.39989864921575602</v>
+      </c>
+    </row>
+    <row r="101" spans="15:23" x14ac:dyDescent="0.25">
+      <c r="O101">
+        <v>1100</v>
+      </c>
+      <c r="P101">
+        <f t="shared" ref="P101:P102" si="18">(O101-998.29)/0.0585</f>
+        <v>1738.6324786324792</v>
+      </c>
+      <c r="R101">
+        <f t="shared" ref="R101:R102" si="19">(O101-964.33)/0.0676</f>
+        <v>2006.9526627218931</v>
+      </c>
+      <c r="S101">
+        <f t="shared" ref="S101:S102" si="20">R101/P101</f>
+        <v>1.1543282938671784</v>
+      </c>
+      <c r="T101">
+        <f t="shared" ref="T101:T102" si="21">(O101-987.67)/0.0643</f>
+        <v>1746.9673405909805</v>
+      </c>
+      <c r="U101">
+        <f t="shared" ref="U101:U102" si="22">T101/P101</f>
+        <v>1.0047939182437551</v>
+      </c>
+      <c r="V101">
+        <f t="shared" ref="V101:V102" si="23">(O101-954.45)/0.0691</f>
+        <v>2106.3675832127346</v>
+      </c>
+      <c r="W101">
+        <f t="shared" ref="W101:W102" si="24">V101/P101</f>
+        <v>1.2115082451867558</v>
+      </c>
+    </row>
+    <row r="102" spans="15:23" x14ac:dyDescent="0.25">
+      <c r="O102">
+        <v>1110</v>
+      </c>
+      <c r="P102">
+        <f t="shared" si="18"/>
+        <v>1909.5726495726501</v>
+      </c>
+      <c r="R102">
+        <f t="shared" si="19"/>
+        <v>2154.8816568047332</v>
+      </c>
+      <c r="S102">
+        <f t="shared" si="20"/>
+        <v>1.1284627779346241</v>
+      </c>
+      <c r="T102">
+        <f t="shared" si="21"/>
+        <v>1902.4883359253506</v>
+      </c>
+      <c r="U102">
+        <f t="shared" si="22"/>
+        <v>0.99629010519768135</v>
+      </c>
+      <c r="V102">
+        <f t="shared" si="23"/>
+        <v>2251.0853835021703</v>
+      </c>
+      <c r="W102">
+        <f t="shared" si="24"/>
+        <v>1.1788424933746031</v>
+      </c>
+    </row>
+    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>23</v>
+      </c>
+      <c r="B118" t="s">
+        <v>24</v>
+      </c>
+      <c r="C118" t="s">
+        <v>3</v>
+      </c>
+      <c r="D118" t="s">
+        <v>16</v>
+      </c>
+      <c r="E118" t="s">
+        <v>25</v>
+      </c>
+      <c r="F118" t="s">
+        <v>3</v>
+      </c>
+      <c r="G118" t="s">
+        <v>16</v>
+      </c>
+      <c r="H118" t="s">
+        <v>26</v>
+      </c>
+      <c r="I118" t="s">
+        <v>3</v>
+      </c>
+      <c r="J118" t="s">
+        <v>16</v>
+      </c>
+      <c r="K118" t="s">
+        <v>27</v>
+      </c>
+      <c r="L118" t="s">
+        <v>3</v>
+      </c>
+      <c r="M118" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>1500</v>
+      </c>
+      <c r="B119">
+        <v>10879</v>
+      </c>
+      <c r="C119">
+        <f>B119*2*PI()/60</f>
+        <v>1139.2462159467786</v>
+      </c>
+      <c r="D119">
+        <f>C119/(A119-781)</f>
+        <v>1.5844870875476755</v>
+      </c>
+      <c r="E119">
+        <v>10633</v>
+      </c>
+      <c r="F119">
+        <f>E119*2*PI()/60</f>
+        <v>1113.4851561873425</v>
+      </c>
+      <c r="G119">
+        <f>F119/(A119-781)</f>
+        <v>1.5486580753648713</v>
+      </c>
+      <c r="H119">
+        <v>10791</v>
+      </c>
+      <c r="I119">
+        <f>H119*2*PI()/60</f>
+        <v>1130.0308774962484</v>
+      </c>
+      <c r="J119">
+        <f>I119/(A119-781)</f>
+        <v>1.5716702051408185</v>
+      </c>
+      <c r="K119">
+        <v>10532</v>
+      </c>
+      <c r="L119">
+        <f>K119*2*PI()/60</f>
+        <v>1102.9084609202569</v>
+      </c>
+      <c r="M119">
+        <f>L119/(A119-781)</f>
+        <v>1.5339477898751834</v>
+      </c>
+    </row>
+    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>1600</v>
+      </c>
+      <c r="B120">
+        <v>10995</v>
+      </c>
+      <c r="C120">
+        <f t="shared" ref="C120:C128" si="25">B120*2*PI()/60</f>
+        <v>1151.3937075406591</v>
+      </c>
+      <c r="D120">
+        <f t="shared" ref="D120:D128" si="26">C120/(A120-781)</f>
+        <v>1.4058531227602675</v>
+      </c>
+      <c r="E120">
+        <v>10787</v>
+      </c>
+      <c r="F120">
+        <f t="shared" ref="F120:F128" si="27">E120*2*PI()/60</f>
+        <v>1129.61199847577</v>
+      </c>
+      <c r="G120">
+        <f t="shared" ref="G120:G128" si="28">F120/(A120-781)</f>
+        <v>1.3792576293965446</v>
+      </c>
+      <c r="H120">
+        <v>10920</v>
+      </c>
+      <c r="I120">
+        <f t="shared" ref="I120:I128" si="29">H120*2*PI()/60</f>
+        <v>1143.5397259066847</v>
+      </c>
+      <c r="J120">
+        <f t="shared" ref="J120:J127" si="30">I120/(A120-781)</f>
+        <v>1.3962634015954636</v>
+      </c>
+      <c r="K120">
+        <v>10664</v>
+      </c>
+      <c r="L120">
+        <f t="shared" ref="L120:L128" si="31">K120*2*PI()/60</f>
+        <v>1116.7314685960519</v>
+      </c>
+      <c r="M120">
+        <f t="shared" ref="M120:M128" si="32">L120/(A120-781)</f>
+        <v>1.3635304866862661</v>
+      </c>
+    </row>
+    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>1700</v>
+      </c>
+      <c r="B121">
+        <v>11082</v>
+      </c>
+      <c r="C121">
+        <f t="shared" si="25"/>
+        <v>1160.5043262360696</v>
+      </c>
+      <c r="D121">
+        <f t="shared" si="26"/>
+        <v>1.2627903441088897</v>
+      </c>
+      <c r="E121">
+        <v>10872</v>
+      </c>
+      <c r="F121">
+        <f t="shared" si="27"/>
+        <v>1138.513177660941</v>
+      </c>
+      <c r="G121">
+        <f t="shared" si="28"/>
+        <v>1.2388609114917748</v>
+      </c>
+      <c r="H121">
+        <v>11020</v>
+      </c>
+      <c r="I121">
+        <f t="shared" si="29"/>
+        <v>1154.0117014186508</v>
+      </c>
+      <c r="J121">
+        <f t="shared" si="30"/>
+        <v>1.2557254640028843</v>
+      </c>
+      <c r="K121">
+        <v>10760</v>
+      </c>
+      <c r="L121">
+        <f t="shared" si="31"/>
+        <v>1126.784565087539</v>
+      </c>
+      <c r="M121">
+        <f t="shared" si="32"/>
+        <v>1.2260985474293133</v>
+      </c>
+    </row>
+    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>1800</v>
+      </c>
+      <c r="B122">
+        <v>11151</v>
+      </c>
+      <c r="C122">
+        <f t="shared" si="25"/>
+        <v>1167.729989339326</v>
+      </c>
+      <c r="D122">
+        <f t="shared" si="26"/>
+        <v>1.1459568099502708</v>
+      </c>
+      <c r="E122">
+        <v>10942</v>
+      </c>
+      <c r="F122">
+        <f t="shared" si="27"/>
+        <v>1145.8435605193174</v>
+      </c>
+      <c r="G122">
+        <f t="shared" si="28"/>
+        <v>1.1244784695969749</v>
+      </c>
+      <c r="H122">
+        <v>11100</v>
+      </c>
+      <c r="I122">
+        <f t="shared" si="29"/>
+        <v>1162.3892818282234</v>
+      </c>
+      <c r="J122">
+        <f t="shared" si="30"/>
+        <v>1.1407156838353516</v>
+      </c>
+      <c r="K122">
+        <v>10835</v>
+      </c>
+      <c r="L122">
+        <f t="shared" si="31"/>
+        <v>1134.6385467215136</v>
+      </c>
+      <c r="M122">
+        <f t="shared" si="32"/>
+        <v>1.1134823814735169</v>
+      </c>
+    </row>
+    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>1900</v>
+      </c>
+      <c r="B123">
+        <v>11208</v>
+      </c>
+      <c r="C123">
+        <f t="shared" si="25"/>
+        <v>1173.6990153811466</v>
+      </c>
+      <c r="D123">
+        <f t="shared" si="26"/>
+        <v>1.0488820512789514</v>
+      </c>
+      <c r="E123">
+        <v>10998</v>
+      </c>
+      <c r="F123">
+        <f t="shared" si="27"/>
+        <v>1151.707866806018</v>
+      </c>
+      <c r="G123">
+        <f t="shared" si="28"/>
+        <v>1.0292295503181572</v>
+      </c>
+      <c r="H123">
+        <v>11155</v>
+      </c>
+      <c r="I123">
+        <f t="shared" si="29"/>
+        <v>1168.1488683598047</v>
+      </c>
+      <c r="J123">
+        <f t="shared" si="30"/>
+        <v>1.0439221343697986</v>
+      </c>
+      <c r="K123">
+        <v>10897</v>
+      </c>
+      <c r="L123">
+        <f t="shared" si="31"/>
+        <v>1141.1311715389324</v>
+      </c>
+      <c r="M123">
+        <f t="shared" si="32"/>
+        <v>1.0197776331893944</v>
+      </c>
+    </row>
+    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>2000</v>
+      </c>
+      <c r="B124">
+        <v>11253</v>
+      </c>
+      <c r="C124">
+        <f t="shared" si="25"/>
+        <v>1178.4114043615314</v>
+      </c>
+      <c r="D124">
+        <f t="shared" si="26"/>
+        <v>0.96670336699059178</v>
+      </c>
+      <c r="E124">
+        <v>11045</v>
+      </c>
+      <c r="F124">
+        <f t="shared" si="27"/>
+        <v>1156.629695296642</v>
+      </c>
+      <c r="G124">
+        <f t="shared" si="28"/>
+        <v>0.94883486078477608</v>
+      </c>
+      <c r="H124">
+        <v>11202</v>
+      </c>
+      <c r="I124">
+        <f t="shared" si="29"/>
+        <v>1173.0706968504287</v>
+      </c>
+      <c r="J124">
+        <f t="shared" si="30"/>
+        <v>0.96232214671897354</v>
+      </c>
+      <c r="K124">
+        <v>10947</v>
+      </c>
+      <c r="L124">
+        <f t="shared" si="31"/>
+        <v>1146.3671592949154</v>
+      </c>
+      <c r="M124">
+        <f t="shared" si="32"/>
+        <v>0.94041604536088219</v>
+      </c>
+    </row>
+    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>2100</v>
+      </c>
+      <c r="B125">
+        <v>11290</v>
+      </c>
+      <c r="C125">
+        <f t="shared" si="25"/>
+        <v>1182.2860353009589</v>
+      </c>
+      <c r="D125">
+        <f t="shared" si="26"/>
+        <v>0.89635029211596584</v>
+      </c>
+      <c r="E125">
+        <v>11084</v>
+      </c>
+      <c r="F125">
+        <f t="shared" si="27"/>
+        <v>1160.713765746309</v>
+      </c>
+      <c r="G125">
+        <f t="shared" si="28"/>
+        <v>0.87999527349985518</v>
+      </c>
+      <c r="H125">
+        <v>11245</v>
+      </c>
+      <c r="I125">
+        <f t="shared" si="29"/>
+        <v>1177.5736463205742</v>
+      </c>
+      <c r="J125">
+        <f t="shared" si="30"/>
+        <v>0.89277759387458244</v>
+      </c>
+      <c r="K125">
+        <v>10989</v>
+      </c>
+      <c r="L125">
+        <f t="shared" si="31"/>
+        <v>1150.7653890099414</v>
+      </c>
+      <c r="M125">
+        <f t="shared" si="32"/>
+        <v>0.87245291054582363</v>
+      </c>
+    </row>
+    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>2200</v>
+      </c>
+      <c r="B126">
+        <v>11323</v>
+      </c>
+      <c r="C126">
+        <f t="shared" si="25"/>
+        <v>1185.7417872199076</v>
+      </c>
+      <c r="D126">
+        <f t="shared" si="26"/>
+        <v>0.83561789092312022</v>
+      </c>
+      <c r="E126">
+        <v>11120</v>
+      </c>
+      <c r="F126">
+        <f t="shared" si="27"/>
+        <v>1164.4836769306166</v>
+      </c>
+      <c r="G126">
+        <f t="shared" si="28"/>
+        <v>0.82063684068401455</v>
+      </c>
+      <c r="H126">
+        <v>11281</v>
+      </c>
+      <c r="I126">
+        <f t="shared" si="29"/>
+        <v>1181.3435575048818</v>
+      </c>
+      <c r="J126">
+        <f t="shared" si="30"/>
+        <v>0.83251836328744311</v>
+      </c>
+      <c r="K126">
+        <v>11028</v>
+      </c>
+      <c r="L126">
+        <f t="shared" si="31"/>
+        <v>1154.8494594596079</v>
+      </c>
+      <c r="M126">
+        <f t="shared" si="32"/>
+        <v>0.81384739919634108</v>
+      </c>
+    </row>
+    <row r="127" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>2300</v>
+      </c>
+      <c r="B127">
+        <v>11468</v>
+      </c>
+      <c r="C127">
+        <f t="shared" si="25"/>
+        <v>1200.9261517122582</v>
+      </c>
+      <c r="D127">
+        <f t="shared" si="26"/>
+        <v>0.79060312818450174</v>
+      </c>
+      <c r="E127">
+        <v>11282</v>
+      </c>
+      <c r="F127">
+        <f t="shared" si="27"/>
+        <v>1181.4482772600015</v>
+      </c>
+      <c r="G127">
+        <f t="shared" si="28"/>
+        <v>0.77778030102699247</v>
+      </c>
+      <c r="H127">
+        <v>11441</v>
+      </c>
+      <c r="I127">
+        <f t="shared" si="29"/>
+        <v>1198.0987183240275</v>
+      </c>
+      <c r="J127">
+        <f t="shared" si="30"/>
+        <v>0.78874175004873437</v>
+      </c>
+      <c r="K127">
+        <v>11194</v>
+      </c>
+      <c r="L127">
+        <f t="shared" si="31"/>
+        <v>1172.2329388094715</v>
+      </c>
+      <c r="M127">
+        <f t="shared" si="32"/>
+        <v>0.77171358710300952</v>
+      </c>
+    </row>
+    <row r="128" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>2400</v>
+      </c>
+      <c r="B128">
+        <v>11469</v>
+      </c>
+      <c r="C128">
+        <f t="shared" si="25"/>
+        <v>1201.0308714673779</v>
+      </c>
+      <c r="D128">
+        <f t="shared" si="26"/>
+        <v>0.74183500399467439</v>
+      </c>
+      <c r="E128">
+        <v>11282</v>
+      </c>
+      <c r="F128">
+        <f t="shared" si="27"/>
+        <v>1181.4482772600015</v>
+      </c>
+      <c r="G128">
+        <f t="shared" si="28"/>
+        <v>0.72973951652872238</v>
+      </c>
+      <c r="H128">
+        <v>11442</v>
+      </c>
+      <c r="I128">
+        <f t="shared" si="29"/>
+        <v>1198.2034380791472</v>
+      </c>
+      <c r="J128">
+        <f>I128/(A128-781)</f>
+        <v>0.74008859671349425</v>
+      </c>
+      <c r="K128">
+        <v>11194</v>
+      </c>
+      <c r="L128">
+        <f t="shared" si="31"/>
+        <v>1172.2329388094715</v>
+      </c>
+      <c r="M128">
+        <f t="shared" si="32"/>
+        <v>0.72404752242709791</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
force/weight data and some other shit
</commit_message>
<xml_diff>
--- a/report/anything else/equation.xlsx
+++ b/report/anything else/equation.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="40">
   <si>
     <t>Input signal</t>
   </si>
@@ -101,6 +101,42 @@
   <si>
     <t>Motor4 RPM</t>
   </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Drone weight:</t>
+  </si>
+  <si>
+    <t>1.427kg</t>
+  </si>
+  <si>
+    <t>Force per motor:</t>
+  </si>
+  <si>
+    <t>~3.5N</t>
+  </si>
+  <si>
+    <t>b~=</t>
+  </si>
+  <si>
+    <t>Motor1</t>
+  </si>
+  <si>
+    <t>Motor2</t>
+  </si>
+  <si>
+    <t>Motor3</t>
+  </si>
+  <si>
+    <t>Motor4</t>
+  </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t>Needed omega ~=</t>
+  </si>
 </sst>
 </file>
 
@@ -118,12 +154,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -138,10 +186,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -528,11 +580,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="84715008"/>
-        <c:axId val="84716544"/>
+        <c:axId val="65644032"/>
+        <c:axId val="65645568"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="84715008"/>
+        <c:axId val="65644032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1200"/>
@@ -545,12 +597,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84716544"/>
+        <c:crossAx val="65645568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="84716544"/>
+        <c:axId val="65645568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10261"/>
@@ -563,13 +615,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84715008"/>
+        <c:crossAx val="65644032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -599,6 +652,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -848,11 +902,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="85531264"/>
-        <c:axId val="85541248"/>
+        <c:axId val="65673856"/>
+        <c:axId val="65683840"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="85531264"/>
+        <c:axId val="65673856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1200"/>
@@ -864,12 +918,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85541248"/>
+        <c:crossAx val="65683840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="85541248"/>
+        <c:axId val="65683840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10261"/>
@@ -882,7 +936,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85531264"/>
+        <c:crossAx val="65673856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -928,6 +982,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1177,11 +1232,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="85570688"/>
-        <c:axId val="85572224"/>
+        <c:axId val="65713280"/>
+        <c:axId val="65714816"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="85570688"/>
+        <c:axId val="65713280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1200"/>
@@ -1193,12 +1248,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85572224"/>
+        <c:crossAx val="65714816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="85572224"/>
+        <c:axId val="65714816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10260"/>
@@ -1211,7 +1266,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85570688"/>
+        <c:crossAx val="65713280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1392,11 +1447,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="88287872"/>
-        <c:axId val="88293760"/>
+        <c:axId val="67971712"/>
+        <c:axId val="67977600"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="88287872"/>
+        <c:axId val="67971712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1406,12 +1461,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88293760"/>
+        <c:crossAx val="67977600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="88293760"/>
+        <c:axId val="67977600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1422,7 +1477,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88287872"/>
+        <c:crossAx val="67971712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1582,11 +1637,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="88308352"/>
-        <c:axId val="88326528"/>
+        <c:axId val="67992192"/>
+        <c:axId val="68010368"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="88308352"/>
+        <c:axId val="67992192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1596,12 +1651,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88326528"/>
+        <c:crossAx val="68010368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="88326528"/>
+        <c:axId val="68010368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1612,7 +1667,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88308352"/>
+        <c:crossAx val="67992192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1815,11 +1870,6 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:trendline>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$A$82:$A$88</c:f>
@@ -1961,11 +2011,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="90333184"/>
-        <c:axId val="90334720"/>
+        <c:axId val="70001792"/>
+        <c:axId val="70003328"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="90333184"/>
+        <c:axId val="70001792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1975,12 +2025,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90334720"/>
+        <c:crossAx val="70003328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="90334720"/>
+        <c:axId val="70003328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1991,7 +2041,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90333184"/>
+        <c:crossAx val="70001792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2205,7 +2255,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$120:$F$126</c:f>
+              <c:f>Sheet1!$G$120:$G$126</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2306,7 +2356,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$I$120:$I$126</c:f>
+              <c:f>Sheet1!$K$120:$K$126</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2407,7 +2457,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$L$120:$L$126</c:f>
+              <c:f>Sheet1!$O$120:$O$126</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2445,11 +2495,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="90393216"/>
-        <c:axId val="90395008"/>
+        <c:axId val="80035840"/>
+        <c:axId val="80037376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="90393216"/>
+        <c:axId val="80035840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2200"/>
@@ -2461,12 +2511,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90395008"/>
+        <c:crossAx val="80037376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="90395008"/>
+        <c:axId val="80037376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1186"/>
@@ -2479,7 +2529,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90393216"/>
+        <c:crossAx val="80035840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2487,6 +2537,387 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>motor1</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.72222222222222221"/>
+                  <c:y val="-0.18481991834354039"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr/>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>M1 = 0.1215x + 957.03</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$119:$A$120</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1600</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$119:$C$120</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1139.2462159467786</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1151.3937075406591</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>motor2</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.54091338582677162"/>
+                  <c:y val="-0.31865594925634294"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr/>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>M2 = 0.0733x + 1013.9</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$121:$A$122</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1700</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1800</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$121:$G$122</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1138.513177660941</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1145.8435605193174</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>motor3</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.65926552930883642"/>
+                  <c:y val="8.1576990376202974E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr/>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>M3 = 0.1047x + 975.99</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$120:$A$121</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1700</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$K$120:$K$121</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1143.5397259066847</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1154.0117014186508</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>motor4</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.23030139982502187"/>
+                  <c:y val="2.63167104111986E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr/>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>M4 = 0.0482x + 1049.7</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$123:$A$125</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1900</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$O$123:$O$125</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1141.1311715389324</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1146.3671592949154</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1150.7653890099414</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="85953536"/>
+        <c:axId val="85950464"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="85953536"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="2000"/>
+          <c:min val="1500"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="85950464"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="85950464"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="85953536"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.72286023622047235"/>
+          <c:y val="0.54070683872849223"/>
+          <c:w val="0.26047309711286087"/>
+          <c:h val="0.45929316127150771"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2708,6 +3139,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>128</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>143</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Chart 9"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3003,10 +3464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W128"/>
+  <dimension ref="A1:W137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A110" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O127" sqref="O127"/>
+    <sheetView tabSelected="1" topLeftCell="D115" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S122" sqref="S122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3015,6 +3476,7 @@
     <col min="2" max="2" width="18.28515625" customWidth="1"/>
     <col min="6" max="6" width="9.140625" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -4675,12 +5137,37 @@
         <v>1.1788424933746031</v>
       </c>
     </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B116" t="s">
+        <v>29</v>
+      </c>
+      <c r="C116" t="s">
+        <v>30</v>
+      </c>
+      <c r="E116" t="s">
+        <v>31</v>
+      </c>
+      <c r="G116" t="s">
+        <v>32</v>
+      </c>
+      <c r="I116" t="s">
+        <v>39</v>
+      </c>
+      <c r="K116" s="5">
+        <v>1144.1400000000001</v>
+      </c>
+      <c r="M116" t="s">
+        <v>33</v>
+      </c>
+      <c r="N116" s="2">
+        <v>2.6699999999999998E-6</v>
+      </c>
+      <c r="O116" s="2"/>
+    </row>
+    <row r="118" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>23</v>
       </c>
@@ -4694,132 +5181,153 @@
         <v>16</v>
       </c>
       <c r="E118" t="s">
+        <v>28</v>
+      </c>
+      <c r="F118" t="s">
         <v>25</v>
       </c>
-      <c r="F118" t="s">
+      <c r="G118" t="s">
         <v>3</v>
       </c>
-      <c r="G118" t="s">
+      <c r="H118" t="s">
         <v>16</v>
       </c>
-      <c r="H118" t="s">
+      <c r="I118" t="s">
+        <v>28</v>
+      </c>
+      <c r="J118" t="s">
         <v>26</v>
       </c>
-      <c r="I118" t="s">
+      <c r="K118" t="s">
         <v>3</v>
       </c>
-      <c r="J118" t="s">
+      <c r="L118" t="s">
         <v>16</v>
       </c>
-      <c r="K118" t="s">
+      <c r="M118" t="s">
+        <v>28</v>
+      </c>
+      <c r="N118" t="s">
         <v>27</v>
       </c>
-      <c r="L118" t="s">
+      <c r="O118" t="s">
         <v>3</v>
       </c>
-      <c r="M118" t="s">
+      <c r="P118" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A119">
+      <c r="Q118" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="119" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A119" s="4">
         <v>1500</v>
       </c>
-      <c r="B119">
+      <c r="B119" s="3">
         <v>10879</v>
       </c>
-      <c r="C119">
+      <c r="C119" s="3">
         <f>B119*2*PI()/60</f>
         <v>1139.2462159467786</v>
       </c>
-      <c r="D119">
+      <c r="D119" s="3">
         <f>C119/(A119-781)</f>
         <v>1.5844870875476755</v>
       </c>
-      <c r="E119">
+      <c r="E119" s="3">
+        <v>3.28</v>
+      </c>
+      <c r="F119">
         <v>10633</v>
       </c>
-      <c r="F119">
-        <f>E119*2*PI()/60</f>
+      <c r="G119">
+        <f>F119*2*PI()/60</f>
         <v>1113.4851561873425</v>
       </c>
-      <c r="G119">
-        <f>F119/(A119-781)</f>
+      <c r="H119">
+        <f>G119/(A119-781)</f>
         <v>1.5486580753648713</v>
       </c>
-      <c r="H119">
+      <c r="J119">
         <v>10791</v>
       </c>
-      <c r="I119">
-        <f>H119*2*PI()/60</f>
+      <c r="K119">
+        <f>J119*2*PI()/60</f>
         <v>1130.0308774962484</v>
       </c>
-      <c r="J119">
-        <f>I119/(A119-781)</f>
+      <c r="L119">
+        <f>K119/(A119-781)</f>
         <v>1.5716702051408185</v>
       </c>
-      <c r="K119">
+      <c r="N119">
         <v>10532</v>
       </c>
-      <c r="L119">
-        <f>K119*2*PI()/60</f>
+      <c r="O119">
+        <f>N119*2*PI()/60</f>
         <v>1102.9084609202569</v>
       </c>
-      <c r="M119">
-        <f>L119/(A119-781)</f>
+      <c r="P119">
+        <f>O119/(A119-781)</f>
         <v>1.5339477898751834</v>
       </c>
     </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A120">
+    <row r="120" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A120" s="4">
         <v>1600</v>
       </c>
-      <c r="B120">
+      <c r="B120" s="3">
         <v>10995</v>
       </c>
-      <c r="C120">
+      <c r="C120" s="3">
         <f t="shared" ref="C120:C128" si="25">B120*2*PI()/60</f>
         <v>1151.3937075406591</v>
       </c>
-      <c r="D120">
+      <c r="D120" s="3">
         <f t="shared" ref="D120:D128" si="26">C120/(A120-781)</f>
         <v>1.4058531227602675</v>
       </c>
-      <c r="E120">
+      <c r="E120" s="3">
+        <v>3.78</v>
+      </c>
+      <c r="F120">
         <v>10787</v>
       </c>
-      <c r="F120">
-        <f t="shared" ref="F120:F128" si="27">E120*2*PI()/60</f>
+      <c r="G120">
+        <f t="shared" ref="G120:G128" si="27">F120*2*PI()/60</f>
         <v>1129.61199847577</v>
       </c>
-      <c r="G120">
-        <f t="shared" ref="G120:G128" si="28">F120/(A120-781)</f>
+      <c r="H120">
+        <f>G120/(A120-781)</f>
         <v>1.3792576293965446</v>
       </c>
-      <c r="H120">
+      <c r="J120" s="3">
         <v>10920</v>
       </c>
-      <c r="I120">
-        <f t="shared" ref="I120:I128" si="29">H120*2*PI()/60</f>
+      <c r="K120" s="3">
+        <f t="shared" ref="K120:K128" si="28">J120*2*PI()/60</f>
         <v>1143.5397259066847</v>
       </c>
-      <c r="J120">
-        <f t="shared" ref="J120:J127" si="30">I120/(A120-781)</f>
+      <c r="L120" s="3">
+        <f>K120/(A120-781)</f>
         <v>1.3962634015954636</v>
       </c>
-      <c r="K120">
+      <c r="M120" s="3">
+        <v>3.4910000000000001</v>
+      </c>
+      <c r="N120">
         <v>10664</v>
       </c>
-      <c r="L120">
-        <f t="shared" ref="L120:L128" si="31">K120*2*PI()/60</f>
+      <c r="O120">
+        <f t="shared" ref="O120:O128" si="29">N120*2*PI()/60</f>
         <v>1116.7314685960519</v>
       </c>
-      <c r="M120">
-        <f t="shared" ref="M120:M128" si="32">L120/(A120-781)</f>
+      <c r="P120">
+        <f>O120/(A120-781)</f>
         <v>1.3635304866862661</v>
       </c>
     </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>1700</v>
       </c>
@@ -4834,41 +5342,47 @@
         <f t="shared" si="26"/>
         <v>1.2627903441088897</v>
       </c>
-      <c r="E121">
+      <c r="F121" s="3">
         <v>10872</v>
       </c>
-      <c r="F121">
+      <c r="G121" s="3">
         <f t="shared" si="27"/>
         <v>1138.513177660941</v>
       </c>
-      <c r="G121">
+      <c r="H121" s="3">
+        <f>G121/(A121-781)</f>
+        <v>1.2388609114917748</v>
+      </c>
+      <c r="I121" s="3">
+        <v>3.46</v>
+      </c>
+      <c r="J121" s="3">
+        <v>11020</v>
+      </c>
+      <c r="K121" s="3">
         <f t="shared" si="28"/>
-        <v>1.2388609114917748</v>
-      </c>
-      <c r="H121">
-        <v>11020</v>
-      </c>
-      <c r="I121">
+        <v>1154.0117014186508</v>
+      </c>
+      <c r="L121" s="3">
+        <f>K121/(A121-781)</f>
+        <v>1.2557254640028843</v>
+      </c>
+      <c r="M121" s="3">
+        <v>3.5550000000000002</v>
+      </c>
+      <c r="N121">
+        <v>10760</v>
+      </c>
+      <c r="O121">
         <f t="shared" si="29"/>
-        <v>1154.0117014186508</v>
-      </c>
-      <c r="J121">
-        <f t="shared" si="30"/>
-        <v>1.2557254640028843</v>
-      </c>
-      <c r="K121">
-        <v>10760</v>
-      </c>
-      <c r="L121">
-        <f t="shared" si="31"/>
         <v>1126.784565087539</v>
       </c>
-      <c r="M121">
-        <f t="shared" si="32"/>
+      <c r="P121">
+        <f>O121/(A121-781)</f>
         <v>1.2260985474293133</v>
       </c>
     </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>1800</v>
       </c>
@@ -4883,41 +5397,44 @@
         <f t="shared" si="26"/>
         <v>1.1459568099502708</v>
       </c>
-      <c r="E122">
+      <c r="F122" s="3">
         <v>10942</v>
       </c>
-      <c r="F122">
+      <c r="G122" s="3">
         <f t="shared" si="27"/>
         <v>1145.8435605193174</v>
       </c>
-      <c r="G122">
+      <c r="H122" s="3">
+        <f>G122/(A122-781)</f>
+        <v>1.1244784695969749</v>
+      </c>
+      <c r="I122" s="3">
+        <v>3.5049999999999999</v>
+      </c>
+      <c r="J122">
+        <v>11100</v>
+      </c>
+      <c r="K122">
         <f t="shared" si="28"/>
-        <v>1.1244784695969749</v>
-      </c>
-      <c r="H122">
-        <v>11100</v>
-      </c>
-      <c r="I122">
+        <v>1162.3892818282234</v>
+      </c>
+      <c r="L122">
+        <f>K122/(A122-781)</f>
+        <v>1.1407156838353516</v>
+      </c>
+      <c r="N122">
+        <v>10835</v>
+      </c>
+      <c r="O122">
         <f t="shared" si="29"/>
-        <v>1162.3892818282234</v>
-      </c>
-      <c r="J122">
-        <f t="shared" si="30"/>
-        <v>1.1407156838353516</v>
-      </c>
-      <c r="K122">
-        <v>10835</v>
-      </c>
-      <c r="L122">
-        <f t="shared" si="31"/>
         <v>1134.6385467215136</v>
       </c>
-      <c r="M122">
-        <f t="shared" si="32"/>
+      <c r="P122">
+        <f>O122/(A122-781)</f>
         <v>1.1134823814735169</v>
       </c>
     </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>1900</v>
       </c>
@@ -4932,41 +5449,44 @@
         <f t="shared" si="26"/>
         <v>1.0488820512789514</v>
       </c>
-      <c r="E123">
+      <c r="F123">
         <v>10998</v>
       </c>
-      <c r="F123">
+      <c r="G123">
         <f t="shared" si="27"/>
         <v>1151.707866806018</v>
       </c>
-      <c r="G123">
+      <c r="H123">
+        <f>G123/(A123-781)</f>
+        <v>1.0292295503181572</v>
+      </c>
+      <c r="J123">
+        <v>11155</v>
+      </c>
+      <c r="K123">
         <f t="shared" si="28"/>
-        <v>1.0292295503181572</v>
-      </c>
-      <c r="H123">
-        <v>11155</v>
-      </c>
-      <c r="I123">
+        <v>1168.1488683598047</v>
+      </c>
+      <c r="L123">
+        <f>K123/(A123-781)</f>
+        <v>1.0439221343697986</v>
+      </c>
+      <c r="N123" s="3">
+        <v>10897</v>
+      </c>
+      <c r="O123" s="3">
         <f t="shared" si="29"/>
-        <v>1168.1488683598047</v>
-      </c>
-      <c r="J123">
-        <f t="shared" si="30"/>
-        <v>1.0439221343697986</v>
-      </c>
-      <c r="K123">
-        <v>10897</v>
-      </c>
-      <c r="L123">
-        <f t="shared" si="31"/>
         <v>1141.1311715389324</v>
       </c>
-      <c r="M123">
-        <f t="shared" si="32"/>
+      <c r="P123" s="3">
+        <f>O123/(A123-781)</f>
         <v>1.0197776331893944</v>
       </c>
-    </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q123" s="3">
+        <v>3.4769999999999999</v>
+      </c>
+    </row>
+    <row r="124" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>2000</v>
       </c>
@@ -4981,41 +5501,44 @@
         <f t="shared" si="26"/>
         <v>0.96670336699059178</v>
       </c>
-      <c r="E124">
+      <c r="F124">
         <v>11045</v>
       </c>
-      <c r="F124">
+      <c r="G124">
         <f t="shared" si="27"/>
         <v>1156.629695296642</v>
       </c>
-      <c r="G124">
+      <c r="H124">
+        <f>G124/(A124-781)</f>
+        <v>0.94883486078477608</v>
+      </c>
+      <c r="J124">
+        <v>11202</v>
+      </c>
+      <c r="K124">
         <f t="shared" si="28"/>
-        <v>0.94883486078477608</v>
-      </c>
-      <c r="H124">
-        <v>11202</v>
-      </c>
-      <c r="I124">
+        <v>1173.0706968504287</v>
+      </c>
+      <c r="L124">
+        <f>K124/(A124-781)</f>
+        <v>0.96232214671897354</v>
+      </c>
+      <c r="N124" s="3">
+        <v>10947</v>
+      </c>
+      <c r="O124" s="3">
         <f t="shared" si="29"/>
-        <v>1173.0706968504287</v>
-      </c>
-      <c r="J124">
-        <f t="shared" si="30"/>
-        <v>0.96232214671897354</v>
-      </c>
-      <c r="K124">
-        <v>10947</v>
-      </c>
-      <c r="L124">
-        <f t="shared" si="31"/>
         <v>1146.3671592949154</v>
       </c>
-      <c r="M124">
-        <f t="shared" si="32"/>
+      <c r="P124" s="3">
+        <f>O124/(A124-781)</f>
         <v>0.94041604536088219</v>
       </c>
-    </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q124" s="3">
+        <v>3.508</v>
+      </c>
+    </row>
+    <row r="125" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>2100</v>
       </c>
@@ -5030,41 +5553,41 @@
         <f t="shared" si="26"/>
         <v>0.89635029211596584</v>
       </c>
-      <c r="E125">
+      <c r="F125">
         <v>11084</v>
       </c>
-      <c r="F125">
+      <c r="G125">
         <f t="shared" si="27"/>
         <v>1160.713765746309</v>
       </c>
-      <c r="G125">
+      <c r="H125">
+        <f>G125/(A125-781)</f>
+        <v>0.87999527349985518</v>
+      </c>
+      <c r="J125">
+        <v>11245</v>
+      </c>
+      <c r="K125">
         <f t="shared" si="28"/>
-        <v>0.87999527349985518</v>
-      </c>
-      <c r="H125">
-        <v>11245</v>
-      </c>
-      <c r="I125">
+        <v>1177.5736463205742</v>
+      </c>
+      <c r="L125">
+        <f>K125/(A125-781)</f>
+        <v>0.89277759387458244</v>
+      </c>
+      <c r="N125">
+        <v>10989</v>
+      </c>
+      <c r="O125">
         <f t="shared" si="29"/>
-        <v>1177.5736463205742</v>
-      </c>
-      <c r="J125">
-        <f t="shared" si="30"/>
-        <v>0.89277759387458244</v>
-      </c>
-      <c r="K125">
-        <v>10989</v>
-      </c>
-      <c r="L125">
-        <f t="shared" si="31"/>
         <v>1150.7653890099414</v>
       </c>
-      <c r="M125">
-        <f t="shared" si="32"/>
+      <c r="P125">
+        <f>O125/(A125-781)</f>
         <v>0.87245291054582363</v>
       </c>
     </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>2200</v>
       </c>
@@ -5079,41 +5602,41 @@
         <f t="shared" si="26"/>
         <v>0.83561789092312022</v>
       </c>
-      <c r="E126">
+      <c r="F126">
         <v>11120</v>
       </c>
-      <c r="F126">
+      <c r="G126">
         <f t="shared" si="27"/>
         <v>1164.4836769306166</v>
       </c>
-      <c r="G126">
+      <c r="H126">
+        <f>G126/(A126-781)</f>
+        <v>0.82063684068401455</v>
+      </c>
+      <c r="J126">
+        <v>11281</v>
+      </c>
+      <c r="K126">
         <f t="shared" si="28"/>
-        <v>0.82063684068401455</v>
-      </c>
-      <c r="H126">
-        <v>11281</v>
-      </c>
-      <c r="I126">
+        <v>1181.3435575048818</v>
+      </c>
+      <c r="L126">
+        <f>K126/(A126-781)</f>
+        <v>0.83251836328744311</v>
+      </c>
+      <c r="N126">
+        <v>11028</v>
+      </c>
+      <c r="O126">
         <f t="shared" si="29"/>
-        <v>1181.3435575048818</v>
-      </c>
-      <c r="J126">
-        <f t="shared" si="30"/>
-        <v>0.83251836328744311</v>
-      </c>
-      <c r="K126">
-        <v>11028</v>
-      </c>
-      <c r="L126">
-        <f t="shared" si="31"/>
         <v>1154.8494594596079</v>
       </c>
-      <c r="M126">
-        <f t="shared" si="32"/>
+      <c r="P126">
+        <f>O126/(A126-781)</f>
         <v>0.81384739919634108</v>
       </c>
     </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>2300</v>
       </c>
@@ -5128,41 +5651,41 @@
         <f t="shared" si="26"/>
         <v>0.79060312818450174</v>
       </c>
-      <c r="E127">
+      <c r="F127">
         <v>11282</v>
       </c>
-      <c r="F127">
+      <c r="G127">
         <f t="shared" si="27"/>
         <v>1181.4482772600015</v>
       </c>
-      <c r="G127">
+      <c r="H127">
+        <f>G127/(A127-781)</f>
+        <v>0.77778030102699247</v>
+      </c>
+      <c r="J127">
+        <v>11441</v>
+      </c>
+      <c r="K127">
         <f t="shared" si="28"/>
-        <v>0.77778030102699247</v>
-      </c>
-      <c r="H127">
-        <v>11441</v>
-      </c>
-      <c r="I127">
+        <v>1198.0987183240275</v>
+      </c>
+      <c r="L127">
+        <f>K127/(A127-781)</f>
+        <v>0.78874175004873437</v>
+      </c>
+      <c r="N127">
+        <v>11194</v>
+      </c>
+      <c r="O127">
         <f t="shared" si="29"/>
-        <v>1198.0987183240275</v>
-      </c>
-      <c r="J127">
-        <f t="shared" si="30"/>
-        <v>0.78874175004873437</v>
-      </c>
-      <c r="K127">
-        <v>11194</v>
-      </c>
-      <c r="L127">
-        <f t="shared" si="31"/>
         <v>1172.2329388094715</v>
       </c>
-      <c r="M127">
-        <f t="shared" si="32"/>
+      <c r="P127">
+        <f>O127/(A127-781)</f>
         <v>0.77171358710300952</v>
       </c>
     </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>2400</v>
       </c>
@@ -5177,38 +5700,98 @@
         <f t="shared" si="26"/>
         <v>0.74183500399467439</v>
       </c>
-      <c r="E128">
+      <c r="F128">
         <v>11282</v>
       </c>
-      <c r="F128">
+      <c r="G128">
         <f t="shared" si="27"/>
         <v>1181.4482772600015</v>
       </c>
-      <c r="G128">
+      <c r="H128">
+        <f>G128/(A128-781)</f>
+        <v>0.72973951652872238</v>
+      </c>
+      <c r="J128">
+        <v>11442</v>
+      </c>
+      <c r="K128">
         <f t="shared" si="28"/>
-        <v>0.72973951652872238</v>
-      </c>
-      <c r="H128">
-        <v>11442</v>
-      </c>
-      <c r="I128">
+        <v>1198.2034380791472</v>
+      </c>
+      <c r="L128">
+        <f>K128/(A128-781)</f>
+        <v>0.74008859671349425</v>
+      </c>
+      <c r="N128">
+        <v>11194</v>
+      </c>
+      <c r="O128">
         <f t="shared" si="29"/>
-        <v>1198.2034380791472</v>
-      </c>
-      <c r="J128">
-        <f>I128/(A128-781)</f>
-        <v>0.74008859671349425</v>
-      </c>
-      <c r="K128">
-        <v>11194</v>
-      </c>
-      <c r="L128">
-        <f t="shared" si="31"/>
         <v>1172.2329388094715</v>
       </c>
-      <c r="M128">
-        <f t="shared" si="32"/>
+      <c r="P128">
+        <f>O128/(A128-781)</f>
         <v>0.72404752242709791</v>
+      </c>
+    </row>
+    <row r="133" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="O133" t="s">
+        <v>38</v>
+      </c>
+      <c r="P133" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="134" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N134" t="s">
+        <v>34</v>
+      </c>
+      <c r="O134" s="6">
+        <f>($K$116-957.03)/0.1215</f>
+        <v>1540.0000000000011</v>
+      </c>
+      <c r="P134" s="6">
+        <f>$K$116/(O134-781)</f>
+        <v>1.5074308300395236</v>
+      </c>
+    </row>
+    <row r="135" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N135" t="s">
+        <v>35</v>
+      </c>
+      <c r="O135" s="6">
+        <f>(K116-1013.9)/0.0733</f>
+        <v>1776.8076398362907</v>
+      </c>
+      <c r="P135" s="6">
+        <f t="shared" ref="P135:P137" si="30">$K$116/(O135-781)</f>
+        <v>1.1489568408895667</v>
+      </c>
+    </row>
+    <row r="136" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N136" t="s">
+        <v>36</v>
+      </c>
+      <c r="O136" s="6">
+        <f>(K116-975.99)/0.1047</f>
+        <v>1606.0171919770783</v>
+      </c>
+      <c r="P136" s="6">
+        <f t="shared" si="30"/>
+        <v>1.3868074642883177</v>
+      </c>
+    </row>
+    <row r="137" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N137" t="s">
+        <v>37</v>
+      </c>
+      <c r="O137" s="6">
+        <f>(K116-1049.7)/0.0482</f>
+        <v>1959.3360995850635</v>
+      </c>
+      <c r="P137" s="6">
+        <f t="shared" si="30"/>
+        <v>0.97097933297884609</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added new stuff, rewritten old stuff, added some dots and shit
</commit_message>
<xml_diff>
--- a/report/anything else/equation.xlsx
+++ b/report/anything else/equation.xlsx
@@ -581,11 +581,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="81569280"/>
-        <c:axId val="81570816"/>
+        <c:axId val="44475904"/>
+        <c:axId val="44477440"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="81569280"/>
+        <c:axId val="44475904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1200"/>
@@ -598,12 +598,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81570816"/>
+        <c:crossAx val="44477440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="81570816"/>
+        <c:axId val="44477440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10261"/>
@@ -616,13 +616,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81569280"/>
+        <c:crossAx val="44475904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -652,6 +653,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -901,11 +903,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="81599104"/>
-        <c:axId val="81613184"/>
+        <c:axId val="44833408"/>
+        <c:axId val="44847488"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="81599104"/>
+        <c:axId val="44833408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1200"/>
@@ -917,12 +919,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81613184"/>
+        <c:crossAx val="44847488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="81613184"/>
+        <c:axId val="44847488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10261"/>
@@ -935,7 +937,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81599104"/>
+        <c:crossAx val="44833408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -981,6 +983,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1230,11 +1233,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="81638528"/>
-        <c:axId val="81640064"/>
+        <c:axId val="44872832"/>
+        <c:axId val="44874368"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="81638528"/>
+        <c:axId val="44872832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1200"/>
@@ -1246,12 +1249,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81640064"/>
+        <c:crossAx val="44874368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="81640064"/>
+        <c:axId val="44874368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10260"/>
@@ -1264,7 +1267,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81638528"/>
+        <c:crossAx val="44872832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1310,6 +1313,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1444,11 +1448,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="86518400"/>
-        <c:axId val="86524288"/>
+        <c:axId val="45820544"/>
+        <c:axId val="45826432"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="86518400"/>
+        <c:axId val="45820544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1458,12 +1462,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86524288"/>
+        <c:crossAx val="45826432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="86524288"/>
+        <c:axId val="45826432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1474,7 +1478,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86518400"/>
+        <c:crossAx val="45820544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1520,6 +1524,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1633,11 +1638,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="86538880"/>
-        <c:axId val="86565248"/>
+        <c:axId val="45841024"/>
+        <c:axId val="45871488"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="86538880"/>
+        <c:axId val="45841024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1647,12 +1652,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86565248"/>
+        <c:crossAx val="45871488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="86565248"/>
+        <c:axId val="45871488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1663,13 +1668,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86538880"/>
+        <c:crossAx val="45841024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2006,11 +2012,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="86451328"/>
-        <c:axId val="86452864"/>
+        <c:axId val="46148608"/>
+        <c:axId val="46158592"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="86451328"/>
+        <c:axId val="46148608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2020,12 +2026,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86452864"/>
+        <c:crossAx val="46158592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="86452864"/>
+        <c:axId val="46158592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2036,13 +2042,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86451328"/>
+        <c:crossAx val="46148608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2489,11 +2496,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="86589440"/>
-        <c:axId val="86590976"/>
+        <c:axId val="46221184"/>
+        <c:axId val="46222720"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="86589440"/>
+        <c:axId val="46221184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2200"/>
@@ -2505,12 +2512,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86590976"/>
+        <c:crossAx val="46222720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="86590976"/>
+        <c:axId val="46222720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1186"/>
@@ -2523,7 +2530,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86589440"/>
+        <c:crossAx val="46221184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2863,11 +2870,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="85990016"/>
-        <c:axId val="85991808"/>
+        <c:axId val="45951616"/>
+        <c:axId val="45953408"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="85990016"/>
+        <c:axId val="45951616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2000"/>
@@ -2879,12 +2886,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85991808"/>
+        <c:crossAx val="45953408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="85991808"/>
+        <c:axId val="45953408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2895,7 +2902,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85990016"/>
+        <c:crossAx val="45951616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3460,8 +3467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P138" sqref="P138"/>
+    <sheetView tabSelected="1" topLeftCell="A127" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P134" sqref="P134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>